<commit_message>
Added the case to aggregate the rows of which the duration is less or equal to 20 ms.
</commit_message>
<xml_diff>
--- a/input_metrics_data/hockey_vlad_metrics_two_tois.xlsx
+++ b/input_metrics_data/hockey_vlad_metrics_two_tois.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shliu03\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\LinkAI - nystart - 2026\Agentic AI platform\Hockey\integration scripts\TPL metrics\tobii_pro_lab_rawFilter_metrics_aois_aggregation\input_metrics_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5742B5-473E-44E8-80DC-755244814B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1B0C87-99C6-4E2E-B6C1-2D8DEAC36CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3EB3ED59-3D8F-4487-93EE-9697D180D6E6}"/>
   </bookViews>
@@ -240,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +420,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -581,11 +587,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1032,7 +1039,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="A10" sqref="A10:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1393,155 +1400,155 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10">
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="2">
         <v>9</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>781</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="2">
         <v>801</v>
       </c>
-      <c r="K10">
-        <v>20</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="K10" s="2">
+        <v>20</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11">
+      <c r="F11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="2">
         <v>10</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>801</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="2">
         <v>821</v>
       </c>
-      <c r="K11">
-        <v>20</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="K11" s="2">
+        <v>20</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12">
+      <c r="F12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="2">
         <v>11</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>821</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="2">
         <v>842</v>
       </c>
-      <c r="K12">
-        <v>20</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="K12" s="2">
+        <v>20</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
+    <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13">
-        <v>12</v>
-      </c>
-      <c r="I13">
+      <c r="F13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="2">
+        <v>12</v>
+      </c>
+      <c r="I13" s="2">
         <v>842</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="2">
         <v>852</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="2">
         <v>10</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The input excel sheet named to be "TPL_raw"
</commit_message>
<xml_diff>
--- a/input_metrics_data/hockey_vlad_metrics_two_tois.xlsx
+++ b/input_metrics_data/hockey_vlad_metrics_two_tois.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\LinkAI - nystart - 2026\Agentic AI platform\Hockey\integration scripts\TPL metrics\tobii_pro_lab_rawFilter_metrics_aois_aggregation\input_metrics_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yl1874\Integration_and_development\non-tobii\tobii_pro_lab_rawFilter_gaze_aois_aggregation\input_metrics_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1B0C87-99C6-4E2E-B6C1-2D8DEAC36CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F8B2B2-60B5-414E-A558-C4AFC50A1546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3EB3ED59-3D8F-4487-93EE-9697D180D6E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{3EB3ED59-3D8F-4487-93EE-9697D180D6E6}"/>
   </bookViews>
   <sheets>
-    <sheet name="TheProblemChild Metrics_two_toi" sheetId="1" r:id="rId1"/>
+    <sheet name="TPL_raw" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -640,74 +640,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -727,7 +659,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="DBEEDD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -1042,23 +974,22 @@
       <selection activeCell="A10" sqref="A10:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" customWidth="1"/>
-    <col min="6" max="6" width="14.08984375" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" customWidth="1"/>
-    <col min="10" max="10" width="11.90625" customWidth="1"/>
-    <col min="11" max="11" width="13.08984375" customWidth="1"/>
-    <col min="12" max="12" width="14.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1096,7 +1027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1134,7 +1065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1172,7 +1103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1141,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1248,7 +1179,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1286,7 +1217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1324,7 +1255,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1362,7 +1293,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +1331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1438,7 +1369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1476,7 +1407,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1514,7 +1445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1552,7 +1483,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1590,7 +1521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1628,7 +1559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1666,7 +1597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1704,7 +1635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1742,7 +1673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1780,7 +1711,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1818,7 +1749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1856,7 +1787,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1894,7 +1825,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1932,7 +1863,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1970,7 +1901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2008,7 +1939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -2046,7 +1977,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -2084,7 +2015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2122,7 +2053,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -2160,7 +2091,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -2198,7 +2129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -2236,7 +2167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -2274,7 +2205,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -2312,7 +2243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -2350,7 +2281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -2388,7 +2319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2426,7 +2357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -2464,7 +2395,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2502,7 +2433,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -2540,7 +2471,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -2578,7 +2509,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2616,7 +2547,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -2654,7 +2585,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2692,7 +2623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -2730,7 +2661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2768,7 +2699,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2806,7 +2737,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -2844,7 +2775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -2882,7 +2813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2920,7 +2851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -2958,7 +2889,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -2996,7 +2927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -3034,7 +2965,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -3072,7 +3003,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -3110,7 +3041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -3148,7 +3079,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -3186,7 +3117,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -3224,7 +3155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -3262,7 +3193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -3300,7 +3231,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -3338,7 +3269,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -3376,7 +3307,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -3414,7 +3345,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -3452,7 +3383,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -3490,7 +3421,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -3528,7 +3459,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -3566,7 +3497,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -3604,7 +3535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -3642,7 +3573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -3680,7 +3611,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -3718,7 +3649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -3756,7 +3687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>12</v>
       </c>
@@ -3794,7 +3725,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -3832,7 +3763,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>12</v>
       </c>
@@ -3870,7 +3801,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>12</v>
       </c>
@@ -3908,7 +3839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>12</v>
       </c>
@@ -3946,7 +3877,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -3984,7 +3915,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>12</v>
       </c>
@@ -4022,7 +3953,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>12</v>
       </c>
@@ -4060,7 +3991,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>12</v>
       </c>
@@ -4098,7 +4029,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>12</v>
       </c>
@@ -4136,7 +4067,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>12</v>
       </c>
@@ -4174,7 +4105,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>12</v>
       </c>
@@ -4212,7 +4143,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>12</v>
       </c>
@@ -4250,7 +4181,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -4288,7 +4219,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>12</v>
       </c>
@@ -4326,7 +4257,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>12</v>
       </c>
@@ -4364,7 +4295,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>12</v>
       </c>
@@ -4402,7 +4333,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -4440,7 +4371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>12</v>
       </c>
@@ -4478,7 +4409,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>12</v>
       </c>
@@ -4516,7 +4447,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>12</v>
       </c>
@@ -4554,7 +4485,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>12</v>
       </c>
@@ -4592,7 +4523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>12</v>
       </c>
@@ -4630,7 +4561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>12</v>
       </c>
@@ -4668,7 +4599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>12</v>
       </c>
@@ -4706,7 +4637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>12</v>
       </c>
@@ -4744,7 +4675,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -4782,7 +4713,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>12</v>
       </c>
@@ -4820,7 +4751,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>12</v>
       </c>

</xml_diff>